<commit_message>
Added experiments with all basins but no boundary conditions
</commit_message>
<xml_diff>
--- a/neuralhydrology/Results_new.xlsx
+++ b/neuralhydrology/Results_new.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="9744"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="9744" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Guerneville" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Hopland" sheetId="3" r:id="rId3"/>
     <sheet name="Calpella" sheetId="4" r:id="rId4"/>
     <sheet name="Guernerville all" sheetId="5" r:id="rId5"/>
+    <sheet name="Guerneville no boundary" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
   <si>
     <t>HMS</t>
   </si>
@@ -82,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +100,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,12 +143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -628,7 +639,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,10 +663,10 @@
         <v>0.73237800399999997</v>
       </c>
       <c r="C2" s="4">
-        <v>0.80282707099999995</v>
+        <v>0.82342129900000005</v>
       </c>
       <c r="D2" s="1">
-        <v>0.85476348599999996</v>
+        <v>0.84428097199999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,11 +676,11 @@
       <c r="B3">
         <v>143219.1079</v>
       </c>
-      <c r="C3" s="1">
-        <v>105517.97440000001</v>
-      </c>
-      <c r="D3" s="4">
-        <v>77723.969729999997</v>
+      <c r="C3" s="4">
+        <v>94496.881580000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>83333.73414</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,10 +691,10 @@
         <v>378.44300490000001</v>
       </c>
       <c r="C4" s="4">
-        <v>324.83530350000001</v>
+        <v>307.40345079999997</v>
       </c>
       <c r="D4" s="1">
-        <v>278.79018939999997</v>
+        <v>288.67582879999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -694,10 +705,10 @@
         <v>0.79119315800000001</v>
       </c>
       <c r="C5" s="4">
-        <v>0.86256915099999998</v>
+        <v>0.91106918699999995</v>
       </c>
       <c r="D5" s="1">
-        <v>0.90929860299999998</v>
+        <v>0.88245241399999996</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,25 +718,25 @@
       <c r="B6">
         <v>1.1795016039999999</v>
       </c>
-      <c r="C6" s="4">
-        <v>1.1086282540000001</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1.0114484379999999</v>
+      <c r="C6" s="1">
+        <v>1.021893969</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.075071036</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>1.037972508</v>
       </c>
       <c r="C7" s="1">
-        <v>0.99006809600000001</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.94536280299999997</v>
+        <v>0.99769417400000004</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0578391629999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -735,11 +746,11 @@
       <c r="B8" s="4">
         <v>1.5442911E-2</v>
       </c>
-      <c r="C8">
-        <v>-4.0391719999999997E-3</v>
+      <c r="C8" s="1">
+        <v>-9.3774899999999998E-4</v>
       </c>
       <c r="D8">
-        <v>-2.2220217E-2</v>
+        <v>2.3522412999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -750,10 +761,10 @@
         <v>0.90031268900000005</v>
       </c>
       <c r="C9" s="4">
-        <v>0.91640276399999998</v>
+        <v>0.91383720800000001</v>
       </c>
       <c r="D9" s="1">
-        <v>0.92851256500000001</v>
+        <v>0.93045572899999995</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -763,11 +774,11 @@
       <c r="B10">
         <v>24.45483673</v>
       </c>
-      <c r="C10" s="4">
-        <v>14.26559219</v>
-      </c>
-      <c r="D10" s="1">
-        <v>4.8824600670000002</v>
+      <c r="C10" s="1">
+        <v>6.5323219999999997</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12.180005189999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -777,25 +788,25 @@
       <c r="B11" s="4">
         <v>25.356068839999999</v>
       </c>
-      <c r="C11">
-        <v>69.393538509999999</v>
+      <c r="C11" s="4">
+        <v>23.833889259999999</v>
       </c>
       <c r="D11" s="1">
-        <v>12.12365756</v>
+        <v>1.2388982719999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>79.444017509999995</v>
       </c>
       <c r="C12" s="4">
-        <v>-2137.4165250000001</v>
-      </c>
-      <c r="D12">
-        <v>-2205.1213750000002</v>
+        <v>-2179.9346439999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8.0069152189999997</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -806,10 +817,10 @@
         <v>0.83333333300000001</v>
       </c>
       <c r="C13" s="1">
+        <v>0.16666666699999999</v>
+      </c>
+      <c r="D13">
         <v>0.5</v>
-      </c>
-      <c r="D13">
-        <v>0.66666666699999999</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -820,10 +831,10 @@
         <v>44.99523319</v>
       </c>
       <c r="C14">
-        <v>58.105471999999999</v>
+        <v>55.327986510000002</v>
       </c>
       <c r="D14">
-        <v>45.448156560000001</v>
+        <v>38.422455480000004</v>
       </c>
     </row>
   </sheetData>
@@ -1038,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1446,4 +1457,212 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.84991477900000001</v>
+      </c>
+      <c r="C2">
+        <v>0.78117591500000005</v>
+      </c>
+      <c r="D2">
+        <v>0.83781096200000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>4623213.6660000002</v>
+      </c>
+      <c r="C3">
+        <v>6740640.3619999997</v>
+      </c>
+      <c r="D3">
+        <v>4996058.71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2150.165962</v>
+      </c>
+      <c r="C4">
+        <v>2596.2743230000001</v>
+      </c>
+      <c r="D4">
+        <v>2235.1865050000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.84303133799999996</v>
+      </c>
+      <c r="C5">
+        <v>0.77070008800000001</v>
+      </c>
+      <c r="D5">
+        <v>0.77274990600000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1.026757235</v>
+      </c>
+      <c r="C6">
+        <v>0.88481617099999998</v>
+      </c>
+      <c r="D6">
+        <v>0.99544427800000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1.1370924179999999</v>
+      </c>
+      <c r="C7">
+        <v>1.1619799200000001</v>
+      </c>
+      <c r="D7">
+        <v>1.2131546639999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>4.8003808000000002E-2</v>
+      </c>
+      <c r="C8">
+        <v>5.6718329999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>7.4637501999999994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.92838379900000001</v>
+      </c>
+      <c r="C9">
+        <v>0.88565997799999996</v>
+      </c>
+      <c r="D9">
+        <v>0.92134289700000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2.5752195759999998</v>
+      </c>
+      <c r="C10">
+        <v>-16.068022389999999</v>
+      </c>
+      <c r="D10">
+        <v>1.085225366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>-24.090634170000001</v>
+      </c>
+      <c r="C11">
+        <v>976.24517149999997</v>
+      </c>
+      <c r="D11">
+        <v>38.799654580000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>97.585158280000002</v>
+      </c>
+      <c r="C12">
+        <v>99.999999990000006</v>
+      </c>
+      <c r="D12">
+        <v>68.906579570000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0.75</v>
+      </c>
+      <c r="C13">
+        <v>0.75</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>14.651639400000001</v>
+      </c>
+      <c r="C14">
+        <v>36.552695409999998</v>
+      </c>
+      <c r="D14">
+        <v>22.49938564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>